<commit_message>
actualizacion excel carga plazas
</commit_message>
<xml_diff>
--- a/public/files/formato_plazas.xlsx
+++ b/public/files/formato_plazas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sigesco\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF282E1-FD7A-45EE-9A65-ADDFDD52B757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A93CBA1-93BA-44EC-9B8B-537B53B9D86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90860A4E-64F2-44A4-B1D4-EE762F1E5817}"/>
+    <workbookView xWindow="5370" yWindow="5370" windowWidth="28800" windowHeight="15345" xr2:uid="{90860A4E-64F2-44A4-B1D4-EE762F1E5817}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuadro_Merito_PUN" sheetId="1" r:id="rId1"/>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -390,7 +390,10 @@
     <t>NIVEL_ID</t>
   </si>
   <si>
-    <t>CODIGO MODULAR</t>
+    <t>ESPECIALIDAD GENERAL</t>
+  </si>
+  <si>
+    <t>BBBBBB</t>
   </si>
 </sst>
 </file>
@@ -806,17 +809,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D75E7D4-6A8F-425A-A88D-398F20941828}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="12" width="19.7109375" customWidth="1"/>
     <col min="13" max="14" width="23.85546875" customWidth="1"/>
@@ -831,13 +834,13 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -878,14 +881,14 @@
       <c r="B2" s="1">
         <v>332342342</v>
       </c>
-      <c r="C2" s="1">
-        <v>5485</v>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>

</xml_diff>